<commit_message>
Add Unit Tests to all IOs. tested and passed.
</commit_message>
<xml_diff>
--- a/Docs/Combination Testing Plan Update.xlsx
+++ b/Docs/Combination Testing Plan Update.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="8070" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="U-1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
   <si>
     <t>PDP-8 Instruction List</t>
   </si>
@@ -297,6 +297,72 @@
   </si>
   <si>
     <t>INPUT = OUTPUT</t>
+  </si>
+  <si>
+    <t>Micro 2</t>
+  </si>
+  <si>
+    <t>Combined Microinstructions Group 2</t>
+  </si>
+  <si>
+    <t>1111| CLA | SMA | SZA | SNL | 0/1 | OSR | HLT | 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       |    2    |   1   |     1    |     1    |    1   |    3   |    3   |</t>
+  </si>
+  <si>
+    <t>SPA SNA</t>
+  </si>
+  <si>
+    <t>SPA SZL</t>
+  </si>
+  <si>
+    <t>SPA SNA SZL</t>
+  </si>
+  <si>
+    <t>SNA SZL</t>
+  </si>
+  <si>
+    <t>SMA SZA</t>
+  </si>
+  <si>
+    <t>SMA SNL</t>
+  </si>
+  <si>
+    <t>SMA SZA SNL</t>
+  </si>
+  <si>
+    <t>SZA SNL</t>
+  </si>
+  <si>
+    <t>OSR HLT</t>
+  </si>
+  <si>
+    <t>SKIP ON POS AC AND SKIP ON NON-ZERO AC</t>
+  </si>
+  <si>
+    <t>SKIP ON POS AC AND SKIP ON ZERO LINK</t>
+  </si>
+  <si>
+    <t>SKIP ON POS AC AD NONZERO AC AND ZERO LINK</t>
+  </si>
+  <si>
+    <t>SKIP ON NONZERO AC AND ZERO LINK</t>
+  </si>
+  <si>
+    <t>SKIP ON MINUZ AC OR NONZERO AC</t>
+  </si>
+  <si>
+    <t>SKIP ON MINUS AC OR NONZERO LINK</t>
+  </si>
+  <si>
+    <t>SKIP ON MINUS AC OR ZERO AC OR NONZERO LINK</t>
+  </si>
+  <si>
+    <t>SKIP ON ZERO AC OR NONZERO LINK</t>
+  </si>
+  <si>
+    <t>OR SWITCH REGISTER WITH AC, HALT</t>
   </si>
 </sst>
 </file>
@@ -400,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -435,6 +501,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,7 +1464,7 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
@@ -1407,7 +1482,7 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>9</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="14" t="s">
@@ -1416,21 +1491,161 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="18">
+        <v>7550</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="18">
+        <v>7530</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="18"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="18">
+        <v>7570</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="18"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="18">
+        <v>7470</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="18"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="18"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="18"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="18">
+        <v>7540</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="18"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="18">
+        <v>7520</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="18"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="18">
+        <v>7560</v>
+      </c>
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="18"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="18">
+        <v>7460</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="18"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="18">
+        <v>7403</v>
+      </c>
+      <c r="C28" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>